<commit_message>
cleaned up seattype and rank prefixes, and removed lowercase letters from seat types
</commit_message>
<xml_diff>
--- a/cut_off_list_2023_24.xlsx
+++ b/cut_off_list_2023_24.xlsx
@@ -571,12 +571,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>GScs</t>
+          <t>GSCS</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>54803,</t>
+          <t>54803</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -771,7 +771,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>GNT2S:</t>
+          <t>GNT2S</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Lscs</t>
+          <t>LSCS</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1071,7 +1071,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>LvJsS</t>
+          <t>LVJSS</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>EWws</t>
+          <t>EWWS</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>GScs</t>
+          <t>GSCS</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1771,7 +1771,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>GNT2S:</t>
+          <t>GNT2S</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1971,7 +1971,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Lscs</t>
+          <t>LSCS</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2471,7 +2471,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>EWws</t>
+          <t>EWWS</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2571,7 +2571,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>GScs</t>
+          <t>GSCS</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2771,7 +2771,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>GNT2S:</t>
+          <t>GNT2S</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -2921,7 +2921,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Lscs</t>
+          <t>LSCS</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -3021,7 +3021,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>LvJS</t>
+          <t>LVJS</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
@@ -3071,7 +3071,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>LNT3S:</t>
+          <t>LNT3S</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -3271,7 +3271,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -3371,7 +3371,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>GScs</t>
+          <t>GSCS</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
@@ -3571,7 +3571,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>GNT2S:</t>
+          <t>GNT2S</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
@@ -3771,12 +3771,12 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Lscs</t>
+          <t>LSCS</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>25655,</t>
+          <t>25655</t>
         </is>
       </c>
       <c r="J67" t="inlineStr">
@@ -3871,7 +3871,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>LvJsS</t>
+          <t>LVJSS</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
@@ -4221,7 +4221,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -4321,7 +4321,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>GScs</t>
+          <t>GSCS</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
@@ -4621,7 +4621,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Lscs</t>
+          <t>LSCS</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
@@ -4871,7 +4871,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I89" t="inlineStr">
@@ -4971,7 +4971,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>GScs</t>
+          <t>GSCS</t>
         </is>
       </c>
       <c r="I91" t="inlineStr">
@@ -5126,7 +5126,7 @@
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>47365,</t>
+          <t>47365</t>
         </is>
       </c>
       <c r="J94" t="inlineStr">
@@ -5171,7 +5171,7 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>GNT2S:</t>
+          <t>GNT2S</t>
         </is>
       </c>
       <c r="I95" t="inlineStr">
@@ -5371,7 +5371,7 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Lscs</t>
+          <t>LSCS</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
@@ -5471,7 +5471,7 @@
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>LvJsS</t>
+          <t>LVJSS</t>
         </is>
       </c>
       <c r="I101" t="inlineStr">
@@ -5671,7 +5671,7 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I105" t="inlineStr">
@@ -6121,7 +6121,7 @@
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>Gsco</t>
+          <t>GSCO</t>
         </is>
       </c>
       <c r="I114" t="inlineStr">
@@ -6271,7 +6271,7 @@
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I117" t="inlineStr">
@@ -7321,7 +7321,7 @@
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I138" t="inlineStr">
@@ -7676,7 +7676,7 @@
       </c>
       <c r="I145" t="inlineStr">
         <is>
-          <t>32855,</t>
+          <t>32855</t>
         </is>
       </c>
       <c r="J145" t="inlineStr">
@@ -8176,7 +8176,7 @@
       </c>
       <c r="I155" t="inlineStr">
         <is>
-          <t>28675,</t>
+          <t>28675</t>
         </is>
       </c>
       <c r="J155" t="inlineStr">
@@ -8321,7 +8321,7 @@
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t>LSCcO</t>
+          <t>LSCCO</t>
         </is>
       </c>
       <c r="I158" t="inlineStr">
@@ -8621,12 +8621,12 @@
       </c>
       <c r="H164" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I164" t="inlineStr">
         <is>
-          <t>27755,</t>
+          <t>27755</t>
         </is>
       </c>
       <c r="J164" t="inlineStr">
@@ -9126,7 +9126,7 @@
       </c>
       <c r="I174" t="inlineStr">
         <is>
-          <t>68446,</t>
+          <t>68446</t>
         </is>
       </c>
       <c r="J174" t="inlineStr">
@@ -9471,7 +9471,7 @@
       </c>
       <c r="H181" t="inlineStr">
         <is>
-          <t>LSco</t>
+          <t>LSCO</t>
         </is>
       </c>
       <c r="I181" t="inlineStr">
@@ -9721,7 +9721,7 @@
       </c>
       <c r="H186" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I186" t="inlineStr">
@@ -10076,7 +10076,7 @@
       </c>
       <c r="I193" t="inlineStr">
         <is>
-          <t>52485,</t>
+          <t>52485</t>
         </is>
       </c>
       <c r="J193" t="inlineStr">
@@ -10571,7 +10571,7 @@
       </c>
       <c r="H203" t="inlineStr">
         <is>
-          <t>LSco</t>
+          <t>LSCO</t>
         </is>
       </c>
       <c r="I203" t="inlineStr">
@@ -10921,7 +10921,7 @@
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I210" t="inlineStr">
@@ -11521,7 +11521,7 @@
       </c>
       <c r="H222" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I222" t="inlineStr">
@@ -12371,7 +12371,7 @@
       </c>
       <c r="H239" t="inlineStr">
         <is>
-          <t>LScO</t>
+          <t>LSCO</t>
         </is>
       </c>
       <c r="I239" t="inlineStr">
@@ -12421,7 +12421,7 @@
       </c>
       <c r="H240" t="inlineStr">
         <is>
-          <t>LvJO</t>
+          <t>LVJO</t>
         </is>
       </c>
       <c r="I240" t="inlineStr">
@@ -12476,7 +12476,7 @@
       </c>
       <c r="I241" t="inlineStr">
         <is>
-          <t>75486,</t>
+          <t>75486</t>
         </is>
       </c>
       <c r="J241" t="inlineStr">
@@ -12621,7 +12621,7 @@
       </c>
       <c r="H244" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I244" t="inlineStr">
@@ -12971,7 +12971,7 @@
       </c>
       <c r="H251" t="inlineStr">
         <is>
-          <t>Gsco</t>
+          <t>GSCO</t>
         </is>
       </c>
       <c r="I251" t="inlineStr">
@@ -13021,7 +13021,7 @@
       </c>
       <c r="H252" t="inlineStr">
         <is>
-          <t>GsTO</t>
+          <t>GSTO</t>
         </is>
       </c>
       <c r="I252" t="inlineStr">
@@ -13071,7 +13071,7 @@
       </c>
       <c r="H253" t="inlineStr">
         <is>
-          <t>Lsco</t>
+          <t>LSCO</t>
         </is>
       </c>
       <c r="I253" t="inlineStr">
@@ -13171,7 +13171,7 @@
       </c>
       <c r="H255" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I255" t="inlineStr">
@@ -13526,7 +13526,7 @@
       </c>
       <c r="I262" t="inlineStr">
         <is>
-          <t>92465,</t>
+          <t>92465</t>
         </is>
       </c>
       <c r="J262" t="inlineStr">
@@ -13671,7 +13671,7 @@
       </c>
       <c r="H265" t="inlineStr">
         <is>
-          <t>Gsco</t>
+          <t>GSCO</t>
         </is>
       </c>
       <c r="I265" t="inlineStr">
@@ -13871,7 +13871,7 @@
       </c>
       <c r="H269" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I269" t="inlineStr">
@@ -14571,7 +14571,7 @@
       </c>
       <c r="H283" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I283" t="inlineStr">
@@ -14676,7 +14676,7 @@
       </c>
       <c r="I285" t="inlineStr">
         <is>
-          <t>66835,</t>
+          <t>66835</t>
         </is>
       </c>
       <c r="J285" t="inlineStr">
@@ -15471,7 +15471,7 @@
       </c>
       <c r="H301" t="inlineStr">
         <is>
-          <t>LSco</t>
+          <t>LSCO</t>
         </is>
       </c>
       <c r="I301" t="inlineStr">
@@ -15571,7 +15571,7 @@
       </c>
       <c r="H303" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I303" t="inlineStr">
@@ -16071,7 +16071,7 @@
       </c>
       <c r="H313" t="inlineStr">
         <is>
-          <t>Gsco</t>
+          <t>GSCO</t>
         </is>
       </c>
       <c r="I313" t="inlineStr">
@@ -16171,7 +16171,7 @@
       </c>
       <c r="H315" t="inlineStr">
         <is>
-          <t>Lsco</t>
+          <t>LSCO</t>
         </is>
       </c>
       <c r="I315" t="inlineStr">
@@ -16221,7 +16221,7 @@
       </c>
       <c r="H316" t="inlineStr">
         <is>
-          <t>LOBcO</t>
+          <t>LOBCO</t>
         </is>
       </c>
       <c r="I316" t="inlineStr">
@@ -16321,7 +16321,7 @@
       </c>
       <c r="H318" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I318" t="inlineStr">
@@ -17171,7 +17171,7 @@
       </c>
       <c r="H335" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I335" t="inlineStr">
@@ -17376,7 +17376,7 @@
       </c>
       <c r="I339" t="inlineStr">
         <is>
-          <t>83545,</t>
+          <t>83545</t>
         </is>
       </c>
       <c r="J339" t="inlineStr">
@@ -17671,7 +17671,7 @@
       </c>
       <c r="H345" t="inlineStr">
         <is>
-          <t>Gsco</t>
+          <t>GSCO</t>
         </is>
       </c>
       <c r="I345" t="inlineStr">
@@ -17821,7 +17821,7 @@
       </c>
       <c r="H348" t="inlineStr">
         <is>
-          <t>Ews</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I348" t="inlineStr">

</xml_diff>

<commit_message>
EWS incorrect seat type issues resolved
</commit_message>
<xml_diff>
--- a/cut_off_list_2023_24.xlsx
+++ b/cut_off_list_2023_24.xlsx
@@ -1471,7 +1471,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>EWWS</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2471,7 +2471,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>EWWS</t>
+          <t>EWS</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">

</xml_diff>

<commit_message>
branch code trimming issues, resolved, patter updated for 9 digits
</commit_message>
<xml_diff>
--- a/cut_off_list_2023_24.xlsx
+++ b/cut_off_list_2023_24.xlsx
@@ -511,7 +511,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -661,7 +661,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -761,7 +761,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -861,7 +861,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -911,7 +911,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1111,7 +1111,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>0219110</t>
+          <t>100219110</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1511,7 +1511,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1611,7 +1611,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1711,7 +1711,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1911,7 +1911,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -2061,7 +2061,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -2111,7 +2111,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -2161,7 +2161,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -2211,7 +2211,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -2261,7 +2261,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -2311,7 +2311,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -2411,7 +2411,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -2461,7 +2461,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>0224610</t>
+          <t>100224610</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -2511,7 +2511,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>0229310</t>
+          <t>100229310</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -2561,7 +2561,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>0229310</t>
+          <t>100229310</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -2611,7 +2611,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>0229310</t>
+          <t>100229310</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>0229310</t>
+          <t>100229310</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>0229310</t>
+          <t>100229310</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -2761,7 +2761,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>0229310</t>
+          <t>100229310</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -2811,7 +2811,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>0229310</t>
+          <t>100229310</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -2861,7 +2861,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>0229310</t>
+          <t>100229310</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -2911,7 +2911,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>0229310</t>
+          <t>100229310</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -2961,7 +2961,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>0229310</t>
+          <t>100229310</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -3011,7 +3011,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>0229310</t>
+          <t>100229310</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>0229310</t>
+          <t>100229310</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -3111,7 +3111,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>0229310</t>
+          <t>100229310</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -3161,7 +3161,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>0229310</t>
+          <t>100229310</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -3211,7 +3211,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>0229310</t>
+          <t>100229310</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -3261,7 +3261,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>0229310</t>
+          <t>100229310</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -3311,7 +3311,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -3361,7 +3361,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -3411,7 +3411,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -3461,7 +3461,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -3511,7 +3511,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
@@ -3611,7 +3611,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -3711,7 +3711,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
@@ -3761,7 +3761,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -3811,7 +3811,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -3861,7 +3861,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -3911,7 +3911,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
@@ -3961,7 +3961,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
@@ -4011,7 +4011,7 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
@@ -4061,7 +4061,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
@@ -4111,7 +4111,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -4161,7 +4161,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -4211,7 +4211,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>0237210</t>
+          <t>100237210</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>0246610</t>
+          <t>100246610</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -4311,7 +4311,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>0246610</t>
+          <t>100246610</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -4361,7 +4361,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>0246610</t>
+          <t>100246610</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -4411,7 +4411,7 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>0246610</t>
+          <t>100246610</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
@@ -4461,7 +4461,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>0246610</t>
+          <t>100246610</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -4511,7 +4511,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>0246610</t>
+          <t>100246610</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -4561,7 +4561,7 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>0246610</t>
+          <t>100246610</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -4611,7 +4611,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>0246610</t>
+          <t>100246610</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -4661,7 +4661,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>0246610</t>
+          <t>100246610</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -4711,7 +4711,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>0246610</t>
+          <t>100246610</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -4761,7 +4761,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>0246610</t>
+          <t>100246610</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -4811,7 +4811,7 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>0246610</t>
+          <t>100246610</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>0246610</t>
+          <t>100246610</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
@@ -4911,7 +4911,7 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>0261210</t>
+          <t>100261210</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
@@ -4961,7 +4961,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>0261210</t>
+          <t>100261210</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
@@ -5011,7 +5011,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>0261210</t>
+          <t>100261210</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
@@ -5061,7 +5061,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>0261210</t>
+          <t>100261210</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
@@ -5111,7 +5111,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>0261210</t>
+          <t>100261210</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
@@ -5161,7 +5161,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>0261210</t>
+          <t>100261210</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
@@ -5211,7 +5211,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>0261210</t>
+          <t>100261210</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
@@ -5261,7 +5261,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>0261210</t>
+          <t>100261210</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
@@ -5311,7 +5311,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>0261210</t>
+          <t>100261210</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
@@ -5361,7 +5361,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>0261210</t>
+          <t>100261210</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
@@ -5411,7 +5411,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>0261210</t>
+          <t>100261210</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
@@ -5461,7 +5461,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>0261210</t>
+          <t>100261210</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
@@ -5511,7 +5511,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>0261210</t>
+          <t>100261210</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
@@ -5561,7 +5561,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>0261210</t>
+          <t>100261210</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
@@ -5611,7 +5611,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>0261210</t>
+          <t>100261210</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
@@ -5661,7 +5661,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>0261210</t>
+          <t>100261210</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
@@ -5711,7 +5711,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>0550310</t>
+          <t>100550310</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
@@ -5761,7 +5761,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>0550310</t>
+          <t>100550310</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
@@ -5811,7 +5811,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>0550310</t>
+          <t>100550310</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
@@ -5861,7 +5861,7 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>0550310</t>
+          <t>100550310</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
@@ -5911,7 +5911,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>0550310</t>
+          <t>100550310</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
@@ -5961,7 +5961,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>0550310</t>
+          <t>100550310</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
@@ -6011,7 +6011,7 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>0550310</t>
+          <t>100550310</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
@@ -6061,7 +6061,7 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>0550310</t>
+          <t>100550310</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
@@ -6111,7 +6111,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>0550310</t>
+          <t>100550310</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
@@ -6161,7 +6161,7 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>0550310</t>
+          <t>100550310</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
@@ -6211,7 +6211,7 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>0550310</t>
+          <t>100550310</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
@@ -6261,7 +6261,7 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>0550310</t>
+          <t>100550310</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
@@ -6311,7 +6311,7 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>0552410</t>
+          <t>100552410</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
@@ -6361,7 +6361,7 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>0552710</t>
+          <t>100552710</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
@@ -6411,7 +6411,7 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
@@ -6461,7 +6461,7 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
@@ -6511,7 +6511,7 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
@@ -6561,7 +6561,7 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
@@ -6611,7 +6611,7 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
@@ -6661,7 +6661,7 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
@@ -6711,7 +6711,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
@@ -6761,7 +6761,7 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
@@ -6811,7 +6811,7 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
@@ -6861,7 +6861,7 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G129" t="inlineStr">
@@ -6911,7 +6911,7 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
@@ -6961,7 +6961,7 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
@@ -7011,7 +7011,7 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
@@ -7061,7 +7061,7 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
@@ -7111,7 +7111,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
@@ -7161,7 +7161,7 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
@@ -7211,7 +7211,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
@@ -7261,7 +7261,7 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G137" t="inlineStr">
@@ -7311,7 +7311,7 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>1219110</t>
+          <t>101219110</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
@@ -7361,7 +7361,7 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
@@ -7411,7 +7411,7 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
@@ -7461,7 +7461,7 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G141" t="inlineStr">
@@ -7511,7 +7511,7 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
@@ -7561,7 +7561,7 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G143" t="inlineStr">
@@ -7611,7 +7611,7 @@
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
@@ -7661,7 +7661,7 @@
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G145" t="inlineStr">
@@ -7711,7 +7711,7 @@
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G146" t="inlineStr">
@@ -7761,7 +7761,7 @@
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G147" t="inlineStr">
@@ -7811,7 +7811,7 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G148" t="inlineStr">
@@ -7861,7 +7861,7 @@
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G149" t="inlineStr">
@@ -7911,7 +7911,7 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G150" t="inlineStr">
@@ -7961,7 +7961,7 @@
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G151" t="inlineStr">
@@ -8011,7 +8011,7 @@
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
@@ -8061,7 +8061,7 @@
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G153" t="inlineStr">
@@ -8111,7 +8111,7 @@
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G154" t="inlineStr">
@@ -8161,7 +8161,7 @@
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G155" t="inlineStr">
@@ -8211,7 +8211,7 @@
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G156" t="inlineStr">
@@ -8261,7 +8261,7 @@
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G157" t="inlineStr">
@@ -8311,7 +8311,7 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
@@ -8361,7 +8361,7 @@
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G159" t="inlineStr">
@@ -8411,7 +8411,7 @@
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G160" t="inlineStr">
@@ -8461,7 +8461,7 @@
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G161" t="inlineStr">
@@ -8511,7 +8511,7 @@
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G162" t="inlineStr">
@@ -8561,7 +8561,7 @@
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G163" t="inlineStr">
@@ -8611,7 +8611,7 @@
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>1224510</t>
+          <t>101224510</t>
         </is>
       </c>
       <c r="G164" t="inlineStr">
@@ -8661,7 +8661,7 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G165" t="inlineStr">
@@ -8711,7 +8711,7 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G166" t="inlineStr">
@@ -8761,7 +8761,7 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G167" t="inlineStr">
@@ -8811,7 +8811,7 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G168" t="inlineStr">
@@ -8861,7 +8861,7 @@
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G169" t="inlineStr">
@@ -8911,7 +8911,7 @@
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G170" t="inlineStr">
@@ -8961,7 +8961,7 @@
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G171" t="inlineStr">
@@ -9011,7 +9011,7 @@
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G172" t="inlineStr">
@@ -9061,7 +9061,7 @@
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G173" t="inlineStr">
@@ -9111,7 +9111,7 @@
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G174" t="inlineStr">
@@ -9161,7 +9161,7 @@
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G175" t="inlineStr">
@@ -9211,7 +9211,7 @@
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G176" t="inlineStr">
@@ -9261,7 +9261,7 @@
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G177" t="inlineStr">
@@ -9311,7 +9311,7 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G178" t="inlineStr">
@@ -9361,7 +9361,7 @@
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G179" t="inlineStr">
@@ -9411,7 +9411,7 @@
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G180" t="inlineStr">
@@ -9461,7 +9461,7 @@
       </c>
       <c r="F181" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G181" t="inlineStr">
@@ -9511,7 +9511,7 @@
       </c>
       <c r="F182" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G182" t="inlineStr">
@@ -9561,7 +9561,7 @@
       </c>
       <c r="F183" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G183" t="inlineStr">
@@ -9611,7 +9611,7 @@
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G184" t="inlineStr">
@@ -9661,7 +9661,7 @@
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G185" t="inlineStr">
@@ -9711,7 +9711,7 @@
       </c>
       <c r="F186" t="inlineStr">
         <is>
-          <t>1229310</t>
+          <t>101229310</t>
         </is>
       </c>
       <c r="G186" t="inlineStr">
@@ -9761,7 +9761,7 @@
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G187" t="inlineStr">
@@ -9811,7 +9811,7 @@
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G188" t="inlineStr">
@@ -9861,7 +9861,7 @@
       </c>
       <c r="F189" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G189" t="inlineStr">
@@ -9911,7 +9911,7 @@
       </c>
       <c r="F190" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G190" t="inlineStr">
@@ -9961,7 +9961,7 @@
       </c>
       <c r="F191" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G191" t="inlineStr">
@@ -10011,7 +10011,7 @@
       </c>
       <c r="F192" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G192" t="inlineStr">
@@ -10061,7 +10061,7 @@
       </c>
       <c r="F193" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G193" t="inlineStr">
@@ -10111,7 +10111,7 @@
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G194" t="inlineStr">
@@ -10161,7 +10161,7 @@
       </c>
       <c r="F195" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G195" t="inlineStr">
@@ -10211,7 +10211,7 @@
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G196" t="inlineStr">
@@ -10261,7 +10261,7 @@
       </c>
       <c r="F197" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G197" t="inlineStr">
@@ -10311,7 +10311,7 @@
       </c>
       <c r="F198" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G198" t="inlineStr">
@@ -10361,7 +10361,7 @@
       </c>
       <c r="F199" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G199" t="inlineStr">
@@ -10411,7 +10411,7 @@
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G200" t="inlineStr">
@@ -10461,7 +10461,7 @@
       </c>
       <c r="F201" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G201" t="inlineStr">
@@ -10511,7 +10511,7 @@
       </c>
       <c r="F202" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G202" t="inlineStr">
@@ -10561,7 +10561,7 @@
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G203" t="inlineStr">
@@ -10611,7 +10611,7 @@
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G204" t="inlineStr">
@@ -10661,7 +10661,7 @@
       </c>
       <c r="F205" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G205" t="inlineStr">
@@ -10711,7 +10711,7 @@
       </c>
       <c r="F206" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G206" t="inlineStr">
@@ -10761,7 +10761,7 @@
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G207" t="inlineStr">
@@ -10811,7 +10811,7 @@
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G208" t="inlineStr">
@@ -10861,7 +10861,7 @@
       </c>
       <c r="F209" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G209" t="inlineStr">
@@ -10911,7 +10911,7 @@
       </c>
       <c r="F210" t="inlineStr">
         <is>
-          <t>1237210</t>
+          <t>101237210</t>
         </is>
       </c>
       <c r="G210" t="inlineStr">
@@ -10961,7 +10961,7 @@
       </c>
       <c r="F211" t="inlineStr">
         <is>
-          <t>1261210</t>
+          <t>101261210</t>
         </is>
       </c>
       <c r="G211" t="inlineStr">
@@ -11011,7 +11011,7 @@
       </c>
       <c r="F212" t="inlineStr">
         <is>
-          <t>1261210</t>
+          <t>101261210</t>
         </is>
       </c>
       <c r="G212" t="inlineStr">
@@ -11061,7 +11061,7 @@
       </c>
       <c r="F213" t="inlineStr">
         <is>
-          <t>1261210</t>
+          <t>101261210</t>
         </is>
       </c>
       <c r="G213" t="inlineStr">
@@ -11111,7 +11111,7 @@
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t>1261210</t>
+          <t>101261210</t>
         </is>
       </c>
       <c r="G214" t="inlineStr">
@@ -11161,7 +11161,7 @@
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t>1261210</t>
+          <t>101261210</t>
         </is>
       </c>
       <c r="G215" t="inlineStr">
@@ -11211,7 +11211,7 @@
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t>1261210</t>
+          <t>101261210</t>
         </is>
       </c>
       <c r="G216" t="inlineStr">
@@ -11261,7 +11261,7 @@
       </c>
       <c r="F217" t="inlineStr">
         <is>
-          <t>1261210</t>
+          <t>101261210</t>
         </is>
       </c>
       <c r="G217" t="inlineStr">
@@ -11311,7 +11311,7 @@
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>1261210</t>
+          <t>101261210</t>
         </is>
       </c>
       <c r="G218" t="inlineStr">
@@ -11361,7 +11361,7 @@
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t>1261210</t>
+          <t>101261210</t>
         </is>
       </c>
       <c r="G219" t="inlineStr">
@@ -11411,7 +11411,7 @@
       </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t>1261210</t>
+          <t>101261210</t>
         </is>
       </c>
       <c r="G220" t="inlineStr">
@@ -11461,7 +11461,7 @@
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t>1261210</t>
+          <t>101261210</t>
         </is>
       </c>
       <c r="G221" t="inlineStr">
@@ -11511,7 +11511,7 @@
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>1261210</t>
+          <t>101261210</t>
         </is>
       </c>
       <c r="G222" t="inlineStr">
@@ -11561,7 +11561,7 @@
       </c>
       <c r="F223" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G223" t="inlineStr">
@@ -11611,7 +11611,7 @@
       </c>
       <c r="F224" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G224" t="inlineStr">
@@ -11661,7 +11661,7 @@
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G225" t="inlineStr">
@@ -11711,7 +11711,7 @@
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G226" t="inlineStr">
@@ -11761,7 +11761,7 @@
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G227" t="inlineStr">
@@ -11811,7 +11811,7 @@
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G228" t="inlineStr">
@@ -11861,7 +11861,7 @@
       </c>
       <c r="F229" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G229" t="inlineStr">
@@ -11911,7 +11911,7 @@
       </c>
       <c r="F230" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G230" t="inlineStr">
@@ -11961,7 +11961,7 @@
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G231" t="inlineStr">
@@ -12011,7 +12011,7 @@
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G232" t="inlineStr">
@@ -12061,7 +12061,7 @@
       </c>
       <c r="F233" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G233" t="inlineStr">
@@ -12111,7 +12111,7 @@
       </c>
       <c r="F234" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G234" t="inlineStr">
@@ -12161,7 +12161,7 @@
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G235" t="inlineStr">
@@ -12211,7 +12211,7 @@
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G236" t="inlineStr">
@@ -12261,7 +12261,7 @@
       </c>
       <c r="F237" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G237" t="inlineStr">
@@ -12311,7 +12311,7 @@
       </c>
       <c r="F238" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G238" t="inlineStr">
@@ -12361,7 +12361,7 @@
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G239" t="inlineStr">
@@ -12411,7 +12411,7 @@
       </c>
       <c r="F240" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G240" t="inlineStr">
@@ -12461,7 +12461,7 @@
       </c>
       <c r="F241" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G241" t="inlineStr">
@@ -12511,7 +12511,7 @@
       </c>
       <c r="F242" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G242" t="inlineStr">
@@ -12561,7 +12561,7 @@
       </c>
       <c r="F243" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G243" t="inlineStr">
@@ -12611,7 +12611,7 @@
       </c>
       <c r="F244" t="inlineStr">
         <is>
-          <t>2124610</t>
+          <t>112124610</t>
         </is>
       </c>
       <c r="G244" t="inlineStr">
@@ -12661,7 +12661,7 @@
       </c>
       <c r="F245" t="inlineStr">
         <is>
-          <t>2137210</t>
+          <t>112137210</t>
         </is>
       </c>
       <c r="G245" t="inlineStr">
@@ -12711,7 +12711,7 @@
       </c>
       <c r="F246" t="inlineStr">
         <is>
-          <t>2137210</t>
+          <t>112137210</t>
         </is>
       </c>
       <c r="G246" t="inlineStr">
@@ -12761,7 +12761,7 @@
       </c>
       <c r="F247" t="inlineStr">
         <is>
-          <t>2137210</t>
+          <t>112137210</t>
         </is>
       </c>
       <c r="G247" t="inlineStr">
@@ -12811,7 +12811,7 @@
       </c>
       <c r="F248" t="inlineStr">
         <is>
-          <t>2137210</t>
+          <t>112137210</t>
         </is>
       </c>
       <c r="G248" t="inlineStr">
@@ -12861,7 +12861,7 @@
       </c>
       <c r="F249" t="inlineStr">
         <is>
-          <t>2137210</t>
+          <t>112137210</t>
         </is>
       </c>
       <c r="G249" t="inlineStr">
@@ -12911,7 +12911,7 @@
       </c>
       <c r="F250" t="inlineStr">
         <is>
-          <t>2137210</t>
+          <t>112137210</t>
         </is>
       </c>
       <c r="G250" t="inlineStr">
@@ -12961,7 +12961,7 @@
       </c>
       <c r="F251" t="inlineStr">
         <is>
-          <t>2137210</t>
+          <t>112137210</t>
         </is>
       </c>
       <c r="G251" t="inlineStr">
@@ -13011,7 +13011,7 @@
       </c>
       <c r="F252" t="inlineStr">
         <is>
-          <t>2137210</t>
+          <t>112137210</t>
         </is>
       </c>
       <c r="G252" t="inlineStr">
@@ -13061,7 +13061,7 @@
       </c>
       <c r="F253" t="inlineStr">
         <is>
-          <t>2137210</t>
+          <t>112137210</t>
         </is>
       </c>
       <c r="G253" t="inlineStr">
@@ -13111,7 +13111,7 @@
       </c>
       <c r="F254" t="inlineStr">
         <is>
-          <t>2137210</t>
+          <t>112137210</t>
         </is>
       </c>
       <c r="G254" t="inlineStr">
@@ -13161,7 +13161,7 @@
       </c>
       <c r="F255" t="inlineStr">
         <is>
-          <t>2137210</t>
+          <t>112137210</t>
         </is>
       </c>
       <c r="G255" t="inlineStr">
@@ -13211,7 +13211,7 @@
       </c>
       <c r="F256" t="inlineStr">
         <is>
-          <t>2161210</t>
+          <t>112161210</t>
         </is>
       </c>
       <c r="G256" t="inlineStr">
@@ -13261,7 +13261,7 @@
       </c>
       <c r="F257" t="inlineStr">
         <is>
-          <t>2161210</t>
+          <t>112161210</t>
         </is>
       </c>
       <c r="G257" t="inlineStr">
@@ -13311,7 +13311,7 @@
       </c>
       <c r="F258" t="inlineStr">
         <is>
-          <t>2161210</t>
+          <t>112161210</t>
         </is>
       </c>
       <c r="G258" t="inlineStr">
@@ -13361,7 +13361,7 @@
       </c>
       <c r="F259" t="inlineStr">
         <is>
-          <t>2161210</t>
+          <t>112161210</t>
         </is>
       </c>
       <c r="G259" t="inlineStr">
@@ -13411,7 +13411,7 @@
       </c>
       <c r="F260" t="inlineStr">
         <is>
-          <t>2161210</t>
+          <t>112161210</t>
         </is>
       </c>
       <c r="G260" t="inlineStr">
@@ -13461,7 +13461,7 @@
       </c>
       <c r="F261" t="inlineStr">
         <is>
-          <t>2161210</t>
+          <t>112161210</t>
         </is>
       </c>
       <c r="G261" t="inlineStr">
@@ -13511,7 +13511,7 @@
       </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t>2161210</t>
+          <t>112161210</t>
         </is>
       </c>
       <c r="G262" t="inlineStr">
@@ -13561,7 +13561,7 @@
       </c>
       <c r="F263" t="inlineStr">
         <is>
-          <t>2161210</t>
+          <t>112161210</t>
         </is>
       </c>
       <c r="G263" t="inlineStr">
@@ -13611,7 +13611,7 @@
       </c>
       <c r="F264" t="inlineStr">
         <is>
-          <t>2161210</t>
+          <t>112161210</t>
         </is>
       </c>
       <c r="G264" t="inlineStr">
@@ -13661,7 +13661,7 @@
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t>2161210</t>
+          <t>112161210</t>
         </is>
       </c>
       <c r="G265" t="inlineStr">
@@ -13711,7 +13711,7 @@
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>2161210</t>
+          <t>112161210</t>
         </is>
       </c>
       <c r="G266" t="inlineStr">
@@ -13761,7 +13761,7 @@
       </c>
       <c r="F267" t="inlineStr">
         <is>
-          <t>2161210</t>
+          <t>112161210</t>
         </is>
       </c>
       <c r="G267" t="inlineStr">
@@ -13811,7 +13811,7 @@
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t>2161210</t>
+          <t>112161210</t>
         </is>
       </c>
       <c r="G268" t="inlineStr">
@@ -13861,7 +13861,7 @@
       </c>
       <c r="F269" t="inlineStr">
         <is>
-          <t>2161210</t>
+          <t>112161210</t>
         </is>
       </c>
       <c r="G269" t="inlineStr">
@@ -13911,7 +13911,7 @@
       </c>
       <c r="F270" t="inlineStr">
         <is>
-          <t>2319110</t>
+          <t>112319110</t>
         </is>
       </c>
       <c r="G270" t="inlineStr">
@@ -13961,7 +13961,7 @@
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>2319110</t>
+          <t>112319110</t>
         </is>
       </c>
       <c r="G271" t="inlineStr">
@@ -14011,7 +14011,7 @@
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>2319110</t>
+          <t>112319110</t>
         </is>
       </c>
       <c r="G272" t="inlineStr">
@@ -14061,7 +14061,7 @@
       </c>
       <c r="F273" t="inlineStr">
         <is>
-          <t>2319110</t>
+          <t>112319110</t>
         </is>
       </c>
       <c r="G273" t="inlineStr">
@@ -14111,7 +14111,7 @@
       </c>
       <c r="F274" t="inlineStr">
         <is>
-          <t>2319110</t>
+          <t>112319110</t>
         </is>
       </c>
       <c r="G274" t="inlineStr">
@@ -14161,7 +14161,7 @@
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>2319110</t>
+          <t>112319110</t>
         </is>
       </c>
       <c r="G275" t="inlineStr">
@@ -14211,7 +14211,7 @@
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>2319110</t>
+          <t>112319110</t>
         </is>
       </c>
       <c r="G276" t="inlineStr">
@@ -14261,7 +14261,7 @@
       </c>
       <c r="F277" t="inlineStr">
         <is>
-          <t>2319110</t>
+          <t>112319110</t>
         </is>
       </c>
       <c r="G277" t="inlineStr">
@@ -14311,7 +14311,7 @@
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>2319110</t>
+          <t>112319110</t>
         </is>
       </c>
       <c r="G278" t="inlineStr">
@@ -14361,7 +14361,7 @@
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>2319110</t>
+          <t>112319110</t>
         </is>
       </c>
       <c r="G279" t="inlineStr">
@@ -14411,7 +14411,7 @@
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>2319110</t>
+          <t>112319110</t>
         </is>
       </c>
       <c r="G280" t="inlineStr">
@@ -14461,7 +14461,7 @@
       </c>
       <c r="F281" t="inlineStr">
         <is>
-          <t>2319110</t>
+          <t>112319110</t>
         </is>
       </c>
       <c r="G281" t="inlineStr">
@@ -14511,7 +14511,7 @@
       </c>
       <c r="F282" t="inlineStr">
         <is>
-          <t>2319110</t>
+          <t>112319110</t>
         </is>
       </c>
       <c r="G282" t="inlineStr">
@@ -14561,7 +14561,7 @@
       </c>
       <c r="F283" t="inlineStr">
         <is>
-          <t>2319110</t>
+          <t>112319110</t>
         </is>
       </c>
       <c r="G283" t="inlineStr">
@@ -14611,7 +14611,7 @@
       </c>
       <c r="F284" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G284" t="inlineStr">
@@ -14661,7 +14661,7 @@
       </c>
       <c r="F285" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G285" t="inlineStr">
@@ -14711,7 +14711,7 @@
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G286" t="inlineStr">
@@ -14761,7 +14761,7 @@
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G287" t="inlineStr">
@@ -14811,7 +14811,7 @@
       </c>
       <c r="F288" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G288" t="inlineStr">
@@ -14861,7 +14861,7 @@
       </c>
       <c r="F289" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G289" t="inlineStr">
@@ -14911,7 +14911,7 @@
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G290" t="inlineStr">
@@ -14961,7 +14961,7 @@
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G291" t="inlineStr">
@@ -15011,7 +15011,7 @@
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G292" t="inlineStr">
@@ -15061,7 +15061,7 @@
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G293" t="inlineStr">
@@ -15111,7 +15111,7 @@
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G294" t="inlineStr">
@@ -15161,7 +15161,7 @@
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G295" t="inlineStr">
@@ -15211,7 +15211,7 @@
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G296" t="inlineStr">
@@ -15261,7 +15261,7 @@
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G297" t="inlineStr">
@@ -15311,7 +15311,7 @@
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G298" t="inlineStr">
@@ -15361,7 +15361,7 @@
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G299" t="inlineStr">
@@ -15411,7 +15411,7 @@
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G300" t="inlineStr">
@@ -15461,7 +15461,7 @@
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G301" t="inlineStr">
@@ -15511,7 +15511,7 @@
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G302" t="inlineStr">
@@ -15561,7 +15561,7 @@
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>2324210</t>
+          <t>112324210</t>
         </is>
       </c>
       <c r="G303" t="inlineStr">
@@ -15611,7 +15611,7 @@
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>2337210</t>
+          <t>112337210</t>
         </is>
       </c>
       <c r="G304" t="inlineStr">
@@ -15661,7 +15661,7 @@
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>2337210</t>
+          <t>112337210</t>
         </is>
       </c>
       <c r="G305" t="inlineStr">
@@ -15711,7 +15711,7 @@
       </c>
       <c r="F306" t="inlineStr">
         <is>
-          <t>2337210</t>
+          <t>112337210</t>
         </is>
       </c>
       <c r="G306" t="inlineStr">
@@ -15761,7 +15761,7 @@
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>2337210</t>
+          <t>112337210</t>
         </is>
       </c>
       <c r="G307" t="inlineStr">
@@ -15811,7 +15811,7 @@
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>2337210</t>
+          <t>112337210</t>
         </is>
       </c>
       <c r="G308" t="inlineStr">
@@ -15861,7 +15861,7 @@
       </c>
       <c r="F309" t="inlineStr">
         <is>
-          <t>2337210</t>
+          <t>112337210</t>
         </is>
       </c>
       <c r="G309" t="inlineStr">
@@ -15911,7 +15911,7 @@
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>2337210</t>
+          <t>112337210</t>
         </is>
       </c>
       <c r="G310" t="inlineStr">
@@ -15961,7 +15961,7 @@
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>2337210</t>
+          <t>112337210</t>
         </is>
       </c>
       <c r="G311" t="inlineStr">
@@ -16011,7 +16011,7 @@
       </c>
       <c r="F312" t="inlineStr">
         <is>
-          <t>2337210</t>
+          <t>112337210</t>
         </is>
       </c>
       <c r="G312" t="inlineStr">
@@ -16061,7 +16061,7 @@
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>2337210</t>
+          <t>112337210</t>
         </is>
       </c>
       <c r="G313" t="inlineStr">
@@ -16111,7 +16111,7 @@
       </c>
       <c r="F314" t="inlineStr">
         <is>
-          <t>2337210</t>
+          <t>112337210</t>
         </is>
       </c>
       <c r="G314" t="inlineStr">
@@ -16161,7 +16161,7 @@
       </c>
       <c r="F315" t="inlineStr">
         <is>
-          <t>2337210</t>
+          <t>112337210</t>
         </is>
       </c>
       <c r="G315" t="inlineStr">
@@ -16211,7 +16211,7 @@
       </c>
       <c r="F316" t="inlineStr">
         <is>
-          <t>2337210</t>
+          <t>112337210</t>
         </is>
       </c>
       <c r="G316" t="inlineStr">
@@ -16261,7 +16261,7 @@
       </c>
       <c r="F317" t="inlineStr">
         <is>
-          <t>2337210</t>
+          <t>112337210</t>
         </is>
       </c>
       <c r="G317" t="inlineStr">
@@ -16311,7 +16311,7 @@
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>2337210</t>
+          <t>112337210</t>
         </is>
       </c>
       <c r="G318" t="inlineStr">
@@ -16361,7 +16361,7 @@
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>2361210</t>
+          <t>112361210</t>
         </is>
       </c>
       <c r="G319" t="inlineStr">
@@ -16411,7 +16411,7 @@
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>2361210</t>
+          <t>112361210</t>
         </is>
       </c>
       <c r="G320" t="inlineStr">
@@ -16461,7 +16461,7 @@
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>2361210</t>
+          <t>112361210</t>
         </is>
       </c>
       <c r="G321" t="inlineStr">
@@ -16511,7 +16511,7 @@
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>2361210</t>
+          <t>112361210</t>
         </is>
       </c>
       <c r="G322" t="inlineStr">
@@ -16561,7 +16561,7 @@
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>2361210</t>
+          <t>112361210</t>
         </is>
       </c>
       <c r="G323" t="inlineStr">
@@ -16611,7 +16611,7 @@
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>2361210</t>
+          <t>112361210</t>
         </is>
       </c>
       <c r="G324" t="inlineStr">
@@ -16661,7 +16661,7 @@
       </c>
       <c r="F325" t="inlineStr">
         <is>
-          <t>2361210</t>
+          <t>112361210</t>
         </is>
       </c>
       <c r="G325" t="inlineStr">
@@ -16711,7 +16711,7 @@
       </c>
       <c r="F326" t="inlineStr">
         <is>
-          <t>2361210</t>
+          <t>112361210</t>
         </is>
       </c>
       <c r="G326" t="inlineStr">
@@ -16761,7 +16761,7 @@
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>2361210</t>
+          <t>112361210</t>
         </is>
       </c>
       <c r="G327" t="inlineStr">
@@ -16811,7 +16811,7 @@
       </c>
       <c r="F328" t="inlineStr">
         <is>
-          <t>2361210</t>
+          <t>112361210</t>
         </is>
       </c>
       <c r="G328" t="inlineStr">
@@ -16861,7 +16861,7 @@
       </c>
       <c r="F329" t="inlineStr">
         <is>
-          <t>2361210</t>
+          <t>112361210</t>
         </is>
       </c>
       <c r="G329" t="inlineStr">
@@ -16911,7 +16911,7 @@
       </c>
       <c r="F330" t="inlineStr">
         <is>
-          <t>2361210</t>
+          <t>112361210</t>
         </is>
       </c>
       <c r="G330" t="inlineStr">
@@ -16961,7 +16961,7 @@
       </c>
       <c r="F331" t="inlineStr">
         <is>
-          <t>2361210</t>
+          <t>112361210</t>
         </is>
       </c>
       <c r="G331" t="inlineStr">
@@ -17011,7 +17011,7 @@
       </c>
       <c r="F332" t="inlineStr">
         <is>
-          <t>2361210</t>
+          <t>112361210</t>
         </is>
       </c>
       <c r="G332" t="inlineStr">
@@ -17061,7 +17061,7 @@
       </c>
       <c r="F333" t="inlineStr">
         <is>
-          <t>2361210</t>
+          <t>112361210</t>
         </is>
       </c>
       <c r="G333" t="inlineStr">
@@ -17111,7 +17111,7 @@
       </c>
       <c r="F334" t="inlineStr">
         <is>
-          <t>2361210</t>
+          <t>112361210</t>
         </is>
       </c>
       <c r="G334" t="inlineStr">
@@ -17161,7 +17161,7 @@
       </c>
       <c r="F335" t="inlineStr">
         <is>
-          <t>2361210</t>
+          <t>112361210</t>
         </is>
       </c>
       <c r="G335" t="inlineStr">
@@ -17211,7 +17211,7 @@
       </c>
       <c r="F336" t="inlineStr">
         <is>
-          <t>2524210</t>
+          <t>112524210</t>
         </is>
       </c>
       <c r="G336" t="inlineStr">
@@ -17261,7 +17261,7 @@
       </c>
       <c r="F337" t="inlineStr">
         <is>
-          <t>2524210</t>
+          <t>112524210</t>
         </is>
       </c>
       <c r="G337" t="inlineStr">
@@ -17311,7 +17311,7 @@
       </c>
       <c r="F338" t="inlineStr">
         <is>
-          <t>2524210</t>
+          <t>112524210</t>
         </is>
       </c>
       <c r="G338" t="inlineStr">
@@ -17361,7 +17361,7 @@
       </c>
       <c r="F339" t="inlineStr">
         <is>
-          <t>2524210</t>
+          <t>112524210</t>
         </is>
       </c>
       <c r="G339" t="inlineStr">
@@ -17411,7 +17411,7 @@
       </c>
       <c r="F340" t="inlineStr">
         <is>
-          <t>2524210</t>
+          <t>112524210</t>
         </is>
       </c>
       <c r="G340" t="inlineStr">
@@ -17461,7 +17461,7 @@
       </c>
       <c r="F341" t="inlineStr">
         <is>
-          <t>2524210</t>
+          <t>112524210</t>
         </is>
       </c>
       <c r="G341" t="inlineStr">
@@ -17511,7 +17511,7 @@
       </c>
       <c r="F342" t="inlineStr">
         <is>
-          <t>2524210</t>
+          <t>112524210</t>
         </is>
       </c>
       <c r="G342" t="inlineStr">
@@ -17561,7 +17561,7 @@
       </c>
       <c r="F343" t="inlineStr">
         <is>
-          <t>2524210</t>
+          <t>112524210</t>
         </is>
       </c>
       <c r="G343" t="inlineStr">
@@ -17611,7 +17611,7 @@
       </c>
       <c r="F344" t="inlineStr">
         <is>
-          <t>2524210</t>
+          <t>112524210</t>
         </is>
       </c>
       <c r="G344" t="inlineStr">
@@ -17661,7 +17661,7 @@
       </c>
       <c r="F345" t="inlineStr">
         <is>
-          <t>2524210</t>
+          <t>112524210</t>
         </is>
       </c>
       <c r="G345" t="inlineStr">
@@ -17711,7 +17711,7 @@
       </c>
       <c r="F346" t="inlineStr">
         <is>
-          <t>2524210</t>
+          <t>112524210</t>
         </is>
       </c>
       <c r="G346" t="inlineStr">
@@ -17761,7 +17761,7 @@
       </c>
       <c r="F347" t="inlineStr">
         <is>
-          <t>2524210</t>
+          <t>112524210</t>
         </is>
       </c>
       <c r="G347" t="inlineStr">
@@ -17811,7 +17811,7 @@
       </c>
       <c r="F348" t="inlineStr">
         <is>
-          <t>2524210</t>
+          <t>112524210</t>
         </is>
       </c>
       <c r="G348" t="inlineStr">
@@ -17861,7 +17861,7 @@
       </c>
       <c r="F349" t="inlineStr">
         <is>
-          <t>2529310</t>
+          <t>112529310</t>
         </is>
       </c>
       <c r="G349" t="inlineStr">
@@ -17911,7 +17911,7 @@
       </c>
       <c r="F350" t="inlineStr">
         <is>
-          <t>2529310</t>
+          <t>112529310</t>
         </is>
       </c>
       <c r="G350" t="inlineStr">
@@ -17961,7 +17961,7 @@
       </c>
       <c r="F351" t="inlineStr">
         <is>
-          <t>2529310</t>
+          <t>112529310</t>
         </is>
       </c>
       <c r="G351" t="inlineStr">
@@ -18011,7 +18011,7 @@
       </c>
       <c r="F352" t="inlineStr">
         <is>
-          <t>2529310</t>
+          <t>112529310</t>
         </is>
       </c>
       <c r="G352" t="inlineStr">
@@ -18061,7 +18061,7 @@
       </c>
       <c r="F353" t="inlineStr">
         <is>
-          <t>2529310</t>
+          <t>112529310</t>
         </is>
       </c>
       <c r="G353" t="inlineStr">
@@ -18111,7 +18111,7 @@
       </c>
       <c r="F354" t="inlineStr">
         <is>
-          <t>2529310</t>
+          <t>112529310</t>
         </is>
       </c>
       <c r="G354" t="inlineStr">
@@ -18161,7 +18161,7 @@
       </c>
       <c r="F355" t="inlineStr">
         <is>
-          <t>2561210</t>
+          <t>112561210</t>
         </is>
       </c>
       <c r="G355" t="inlineStr">

</xml_diff>